<commit_message>
LMDI: Versjon 1.0.6 6e05e801b0fc67a31d9121f33125496b6f7ed95a
</commit_message>
<xml_diff>
--- a/currentbuild/ValueSet-atc-valueset.xlsx
+++ b/currentbuild/ValueSet-atc-valueset.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Property</t>
   </si>
@@ -54,13 +54,10 @@
     <t>Experimental</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-11</t>
+    <t>2025-09-12</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -310,76 +307,74 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>14</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>16</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>18</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s" s="2">
         <v>23</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s" s="2">
         <v>27</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -401,28 +396,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>32</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>